<commit_message>
Revise and align project documentation
</commit_message>
<xml_diff>
--- a/docs/08.10.25/gannt_chart.xlsx
+++ b/docs/08.10.25/gannt_chart.xlsx
@@ -180,11 +180,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1745046396"/>
-        <c:axId val="1726665277"/>
+        <c:axId val="606408572"/>
+        <c:axId val="2004527508"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1745046396"/>
+        <c:axId val="606408572"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -236,10 +236,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1726665277"/>
+        <c:crossAx val="2004527508"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1726665277"/>
+        <c:axId val="2004527508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -314,7 +314,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1745046396"/>
+        <c:crossAx val="606408572"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -410,11 +410,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="295621550"/>
-        <c:axId val="2048480418"/>
+        <c:axId val="1464831156"/>
+        <c:axId val="1152518487"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="295621550"/>
+        <c:axId val="1464831156"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -466,10 +466,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2048480418"/>
+        <c:crossAx val="1152518487"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2048480418"/>
+        <c:axId val="1152518487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +544,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295621550"/>
+        <c:crossAx val="1464831156"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>

</xml_diff>